<commit_message>
penambahan master valuta dan negara dan kota
</commit_message>
<xml_diff>
--- a/Nita Doc/Dokumentasi.xlsx
+++ b/Nita Doc/Dokumentasi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="750" windowWidth="19815" windowHeight="7245" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="750" windowWidth="19815" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kode Table" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Kode</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>HTTRX020</t>
+  </si>
+  <si>
+    <t>MST040</t>
+  </si>
+  <si>
+    <t>Negara</t>
+  </si>
+  <si>
+    <t>MST041</t>
+  </si>
+  <si>
+    <t>Kota</t>
   </si>
 </sst>
 </file>
@@ -601,10 +613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -676,6 +688,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -685,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>